<commit_message>
chore: restore local changes
</commit_message>
<xml_diff>
--- a/adapt-design-files/adapt_基本設計_最終版.xlsx
+++ b/adapt-design-files/adapt_基本設計_最終版.xlsx
@@ -31883,17 +31883,17 @@
       </c>
       <c r="C32" s="44" t="inlineStr">
         <is>
-          <t>/api/v1/instructor/analytics/overview</t>
+          <t>/api/v1/instructor/courses/{courseId}/publish</t>
         </is>
       </c>
       <c r="D32" s="43" t="inlineStr">
         <is>
-          <t>GET</t>
+          <t>POST</t>
         </is>
       </c>
       <c r="E32" s="44" t="inlineStr">
         <is>
-          <t>売上分析サマリ</t>
+          <t>コース公開（講師）</t>
         </is>
       </c>
       <c r="F32" s="43" t="inlineStr">
@@ -31903,12 +31903,12 @@
       </c>
       <c r="G32" s="44" t="inlineStr">
         <is>
-          <t>instructor</t>
+          <t>instructor_owner</t>
         </is>
       </c>
       <c r="H32" s="43" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>AUDIT_LOG</t>
         </is>
       </c>
       <c r="I32" s="45" t="inlineStr">
@@ -31918,22 +31918,22 @@
       </c>
       <c r="J32" s="45" t="inlineStr">
         <is>
-          <t>GenericListResponse</t>
+          <t>CourseDetailView</t>
         </is>
       </c>
       <c r="K32" s="45" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>200, 403, 423</t>
         </is>
       </c>
       <c r="L32" s="45" t="inlineStr">
         <is>
-          <t>KEEP</t>
+          <t>v1.2</t>
         </is>
       </c>
       <c r="M32" s="45" t="inlineStr">
         <is>
-          <t>期間別の収益、成約率、受講生離脱ポイント等の分析サマリーを取得。</t>
+          <t>ownerUserId一致の講師がコースを公開。statusをactiveに変更。operator作成コースの場合、CourseMember.role=instructor→instructor_ownerへ昇格（委譲完了）。</t>
         </is>
       </c>
     </row>
@@ -31948,17 +31948,17 @@
       </c>
       <c r="C33" s="44" t="inlineStr">
         <is>
-          <t>/api/v1/instructor/settings/payout</t>
+          <t>/api/v1/instructor/analytics/overview</t>
         </is>
       </c>
       <c r="D33" s="43" t="inlineStr">
         <is>
-          <t>PUT</t>
+          <t>GET</t>
         </is>
       </c>
       <c r="E33" s="44" t="inlineStr">
         <is>
-          <t>振込先銀行設定</t>
+          <t>売上分析サマリ</t>
         </is>
       </c>
       <c r="F33" s="43" t="inlineStr">
@@ -31968,7 +31968,7 @@
       </c>
       <c r="G33" s="44" t="inlineStr">
         <is>
-          <t>instructor_owner</t>
+          <t>instructor</t>
         </is>
       </c>
       <c r="H33" s="43" t="inlineStr">
@@ -31978,12 +31978,12 @@
       </c>
       <c r="I33" s="45" t="inlineStr">
         <is>
-          <t>GenericWriteRequest</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J33" s="45" t="inlineStr">
         <is>
-          <t>SuccessResponse</t>
+          <t>GenericListResponse</t>
         </is>
       </c>
       <c r="K33" s="45" t="inlineStr">
@@ -31998,7 +31998,7 @@
       </c>
       <c r="M33" s="45" t="inlineStr">
         <is>
-          <t>講師への報酬振込先口座情報をStripe Connect等と連携して設定・更新。</t>
+          <t>期間別の収益、成約率、受講生離脱ポイント等の分析サマリーを取得。</t>
         </is>
       </c>
     </row>
@@ -32013,17 +32013,17 @@
       </c>
       <c r="C34" s="44" t="inlineStr">
         <is>
-          <t>/api/v1/instructor/courses/{courseId}/syllabus</t>
+          <t>/api/v1/instructor/settings/payout</t>
         </is>
       </c>
       <c r="D34" s="43" t="inlineStr">
         <is>
-          <t>GET</t>
+          <t>PUT</t>
         </is>
       </c>
       <c r="E34" s="44" t="inlineStr">
         <is>
-          <t>シラバス構造取得</t>
+          <t>振込先銀行設定</t>
         </is>
       </c>
       <c r="F34" s="43" t="inlineStr">
@@ -32033,7 +32033,7 @@
       </c>
       <c r="G34" s="44" t="inlineStr">
         <is>
-          <t>instructor</t>
+          <t>instructor_owner</t>
         </is>
       </c>
       <c r="H34" s="43" t="inlineStr">
@@ -32043,12 +32043,12 @@
       </c>
       <c r="I34" s="45" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>GenericWriteRequest</t>
         </is>
       </c>
       <c r="J34" s="45" t="inlineStr">
         <is>
-          <t>CourseDetailView</t>
+          <t>SuccessResponse</t>
         </is>
       </c>
       <c r="K34" s="45" t="inlineStr">
@@ -32063,7 +32063,7 @@
       </c>
       <c r="M34" s="45" t="inlineStr">
         <is>
-          <t>編集中の章立てとレッスン構成をツリー形式で取得（image_32dd18の構成用）。</t>
+          <t>講師への報酬振込先口座情報をStripe Connect等と連携して設定・更新。</t>
         </is>
       </c>
     </row>
@@ -32078,17 +32078,17 @@
       </c>
       <c r="C35" s="44" t="inlineStr">
         <is>
-          <t>/api/v1/instructor/courses/{courseId}/sections</t>
+          <t>/api/v1/instructor/courses/{courseId}/syllabus</t>
         </is>
       </c>
       <c r="D35" s="43" t="inlineStr">
         <is>
-          <t>POST</t>
+          <t>GET</t>
         </is>
       </c>
       <c r="E35" s="44" t="inlineStr">
         <is>
-          <t>セクション追加</t>
+          <t>シラバス構造取得</t>
         </is>
       </c>
       <c r="F35" s="43" t="inlineStr">
@@ -32103,12 +32103,12 @@
       </c>
       <c r="H35" s="43" t="inlineStr">
         <is>
-          <t>423_ON_FROZEN</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I35" s="45" t="inlineStr">
         <is>
-          <t>GenericWriteRequest</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J35" s="45" t="inlineStr">
@@ -32118,7 +32118,7 @@
       </c>
       <c r="K35" s="45" t="inlineStr">
         <is>
-          <t>201, 423</t>
+          <t>200</t>
         </is>
       </c>
       <c r="L35" s="45" t="inlineStr">
@@ -32128,7 +32128,7 @@
       </c>
       <c r="M35" s="45" t="inlineStr">
         <is>
-          <t>カリキュラム内に新しい「章」を追加。423チェック対象。</t>
+          <t>編集中の章立てとレッスン構成をツリー形式で取得（image_32dd18の構成用）。</t>
         </is>
       </c>
     </row>
@@ -32143,17 +32143,17 @@
       </c>
       <c r="C36" s="44" t="inlineStr">
         <is>
-          <t>/api/v1/instructor/sections/{sectionId}</t>
+          <t>/api/v1/instructor/courses/{courseId}/sections</t>
         </is>
       </c>
       <c r="D36" s="43" t="inlineStr">
         <is>
-          <t>PUT</t>
+          <t>POST</t>
         </is>
       </c>
       <c r="E36" s="44" t="inlineStr">
         <is>
-          <t>セクション編集</t>
+          <t>セクション追加</t>
         </is>
       </c>
       <c r="F36" s="43" t="inlineStr">
@@ -32178,12 +32178,12 @@
       </c>
       <c r="J36" s="45" t="inlineStr">
         <is>
-          <t>SuccessResponse</t>
+          <t>CourseDetailView</t>
         </is>
       </c>
       <c r="K36" s="45" t="inlineStr">
         <is>
-          <t>200, 423</t>
+          <t>201, 423</t>
         </is>
       </c>
       <c r="L36" s="45" t="inlineStr">
@@ -32193,7 +32193,7 @@
       </c>
       <c r="M36" s="45" t="inlineStr">
         <is>
-          <t>セクション名の変更、表示順の並び替え、および削除。</t>
+          <t>カリキュラム内に新しい「章」を追加。423チェック対象。</t>
         </is>
       </c>
     </row>
@@ -32213,12 +32213,12 @@
       </c>
       <c r="D37" s="43" t="inlineStr">
         <is>
-          <t>DELETE</t>
+          <t>PUT</t>
         </is>
       </c>
       <c r="E37" s="44" t="inlineStr">
         <is>
-          <t>セクション削除</t>
+          <t>セクション編集</t>
         </is>
       </c>
       <c r="F37" s="43" t="inlineStr">
@@ -32238,7 +32238,7 @@
       </c>
       <c r="I37" s="45" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>GenericWriteRequest</t>
         </is>
       </c>
       <c r="J37" s="45" t="inlineStr">
@@ -32258,7 +32258,7 @@
       </c>
       <c r="M37" s="45" t="inlineStr">
         <is>
-          <t>指定されたセクションと、配下のレッスン紐付けを削除（論理/物理）。</t>
+          <t>セクション名の変更、表示順の並び替え、および削除。</t>
         </is>
       </c>
     </row>
@@ -32273,17 +32273,17 @@
       </c>
       <c r="C38" s="44" t="inlineStr">
         <is>
-          <t>/api/v1/instructor/sections/{sectionId}/lessons</t>
+          <t>/api/v1/instructor/sections/{sectionId}</t>
         </is>
       </c>
       <c r="D38" s="43" t="inlineStr">
         <is>
-          <t>POST</t>
+          <t>DELETE</t>
         </is>
       </c>
       <c r="E38" s="44" t="inlineStr">
         <is>
-          <t>レッスン作成</t>
+          <t>セクション削除</t>
         </is>
       </c>
       <c r="F38" s="43" t="inlineStr">
@@ -32303,7 +32303,7 @@
       </c>
       <c r="I38" s="45" t="inlineStr">
         <is>
-          <t>GenericWriteRequest</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J38" s="45" t="inlineStr">
@@ -32313,7 +32313,7 @@
       </c>
       <c r="K38" s="45" t="inlineStr">
         <is>
-          <t>201, 423</t>
+          <t>200, 423</t>
         </is>
       </c>
       <c r="L38" s="45" t="inlineStr">
@@ -32323,7 +32323,7 @@
       </c>
       <c r="M38" s="45" t="inlineStr">
         <is>
-          <t>指定セクションに新規レッスンを追加（座学/動画/課題/ライブ）（image_32dcf8反映）。</t>
+          <t>指定されたセクションと、配下のレッスン紐付けを削除（論理/物理）。</t>
         </is>
       </c>
     </row>
@@ -32338,17 +32338,17 @@
       </c>
       <c r="C39" s="44" t="inlineStr">
         <is>
-          <t>/api/v1/instructor/lessons/{lessonId}</t>
+          <t>/api/v1/instructor/sections/{sectionId}/lessons</t>
         </is>
       </c>
       <c r="D39" s="43" t="inlineStr">
         <is>
-          <t>GET</t>
+          <t>POST</t>
         </is>
       </c>
       <c r="E39" s="44" t="inlineStr">
         <is>
-          <t>レッスン詳細取得</t>
+          <t>レッスン作成</t>
         </is>
       </c>
       <c r="F39" s="43" t="inlineStr">
@@ -32363,22 +32363,22 @@
       </c>
       <c r="H39" s="43" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>423_ON_FROZEN</t>
         </is>
       </c>
       <c r="I39" s="45" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>GenericWriteRequest</t>
         </is>
       </c>
       <c r="J39" s="45" t="inlineStr">
         <is>
-          <t>GenericDetailView</t>
+          <t>SuccessResponse</t>
         </is>
       </c>
       <c r="K39" s="45" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>201, 423</t>
         </is>
       </c>
       <c r="L39" s="45" t="inlineStr">
@@ -32388,7 +32388,7 @@
       </c>
       <c r="M39" s="45" t="inlineStr">
         <is>
-          <t>編集画面用。動画URL、リッチテキスト本文、課題要件、Drip設定の詳細。</t>
+          <t>指定セクションに新規レッスンを追加（座学/動画/課題/ライブ）（image_32dcf8反映）。</t>
         </is>
       </c>
     </row>
@@ -32408,12 +32408,12 @@
       </c>
       <c r="D40" s="43" t="inlineStr">
         <is>
-          <t>PUT</t>
+          <t>GET</t>
         </is>
       </c>
       <c r="E40" s="44" t="inlineStr">
         <is>
-          <t>レッスン編集</t>
+          <t>レッスン詳細取得</t>
         </is>
       </c>
       <c r="F40" s="43" t="inlineStr">
@@ -32428,22 +32428,22 @@
       </c>
       <c r="H40" s="43" t="inlineStr">
         <is>
-          <t>423_ON_FROZEN</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I40" s="45" t="inlineStr">
         <is>
-          <t>GenericWriteRequest</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J40" s="45" t="inlineStr">
         <is>
-          <t>SuccessResponse</t>
+          <t>GenericDetailView</t>
         </is>
       </c>
       <c r="K40" s="45" t="inlineStr">
         <is>
-          <t>200, 423</t>
+          <t>200</t>
         </is>
       </c>
       <c r="L40" s="45" t="inlineStr">
@@ -32453,7 +32453,7 @@
       </c>
       <c r="M40" s="45" t="inlineStr">
         <is>
-          <t>コンテンツの修正、Drip(解禁日)、先行ロック条件の保存。423チェック対象。</t>
+          <t>編集画面用。動画URL、リッチテキスト本文、課題要件、Drip設定の詳細。</t>
         </is>
       </c>
     </row>
@@ -32473,12 +32473,12 @@
       </c>
       <c r="D41" s="43" t="inlineStr">
         <is>
-          <t>DELETE</t>
+          <t>PUT</t>
         </is>
       </c>
       <c r="E41" s="44" t="inlineStr">
         <is>
-          <t>レッスン削除</t>
+          <t>レッスン編集</t>
         </is>
       </c>
       <c r="F41" s="43" t="inlineStr">
@@ -32498,7 +32498,7 @@
       </c>
       <c r="I41" s="45" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>GenericWriteRequest</t>
         </is>
       </c>
       <c r="J41" s="45" t="inlineStr">
@@ -32518,7 +32518,7 @@
       </c>
       <c r="M41" s="45" t="inlineStr">
         <is>
-          <t>レッスンをカリキュラムから削除。</t>
+          <t>コンテンツの修正、Drip(解禁日)、先行ロック条件の保存。423チェック対象。</t>
         </is>
       </c>
     </row>
@@ -32533,17 +32533,17 @@
       </c>
       <c r="C42" s="44" t="inlineStr">
         <is>
-          <t>/api/v1/instructor/lessons/{lessonId}/live</t>
+          <t>/api/v1/instructor/lessons/{lessonId}</t>
         </is>
       </c>
       <c r="D42" s="43" t="inlineStr">
         <is>
-          <t>PUT</t>
+          <t>DELETE</t>
         </is>
       </c>
       <c r="E42" s="44" t="inlineStr">
         <is>
-          <t>ライブ配信設定</t>
+          <t>レッスン削除</t>
         </is>
       </c>
       <c r="F42" s="43" t="inlineStr">
@@ -32563,7 +32563,7 @@
       </c>
       <c r="I42" s="45" t="inlineStr">
         <is>
-          <t>GenericWriteRequest</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J42" s="45" t="inlineStr">
@@ -32583,7 +32583,7 @@
       </c>
       <c r="M42" s="45" t="inlineStr">
         <is>
-          <t>ZoomやYouTube LiveのURL、および配信日時の設定（カレンダー連動）。</t>
+          <t>レッスンをカリキュラムから削除。</t>
         </is>
       </c>
     </row>
@@ -32598,17 +32598,17 @@
       </c>
       <c r="C43" s="44" t="inlineStr">
         <is>
-          <t>/api/v1/instructor/courses/{courseId}/submissions</t>
+          <t>/api/v1/instructor/lessons/{lessonId}/live</t>
         </is>
       </c>
       <c r="D43" s="43" t="inlineStr">
         <is>
-          <t>GET</t>
+          <t>PUT</t>
         </is>
       </c>
       <c r="E43" s="44" t="inlineStr">
         <is>
-          <t>提出一覧取得</t>
+          <t>ライブ配信設定</t>
         </is>
       </c>
       <c r="F43" s="43" t="inlineStr">
@@ -32623,22 +32623,22 @@
       </c>
       <c r="H43" s="43" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>423_ON_FROZEN</t>
         </is>
       </c>
       <c r="I43" s="45" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>GenericWriteRequest</t>
         </is>
       </c>
       <c r="J43" s="45" t="inlineStr">
         <is>
-          <t>CourseDetailView</t>
+          <t>SuccessResponse</t>
         </is>
       </c>
       <c r="K43" s="45" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>200, 423</t>
         </is>
       </c>
       <c r="L43" s="45" t="inlineStr">
@@ -32648,7 +32648,7 @@
       </c>
       <c r="M43" s="45" t="inlineStr">
         <is>
-          <t>受講者別の課題進捗、未確認提出物、最終提出日時の一覧（image_32dcd7反映）。</t>
+          <t>ZoomやYouTube LiveのURL、および配信日時の設定（カレンダー連動）。</t>
         </is>
       </c>
     </row>
@@ -32663,17 +32663,17 @@
       </c>
       <c r="C44" s="44" t="inlineStr">
         <is>
-          <t>/api/v1/instructor/submissions/{submissionId}/evaluation</t>
+          <t>/api/v1/instructor/courses/{courseId}/submissions</t>
         </is>
       </c>
       <c r="D44" s="43" t="inlineStr">
         <is>
-          <t>PATCH</t>
+          <t>GET</t>
         </is>
       </c>
       <c r="E44" s="44" t="inlineStr">
         <is>
-          <t>評価・採点実行</t>
+          <t>提出一覧取得</t>
         </is>
       </c>
       <c r="F44" s="43" t="inlineStr">
@@ -32683,22 +32683,22 @@
       </c>
       <c r="G44" s="44" t="inlineStr">
         <is>
-          <t>instructor, assistant</t>
+          <t>instructor</t>
         </is>
       </c>
       <c r="H44" s="43" t="inlineStr">
         <is>
-          <t>THREAD_REPLY(AUTO)</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I44" s="45" t="inlineStr">
         <is>
-          <t>GenericWriteRequest</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J44" s="45" t="inlineStr">
         <is>
-          <t>SubmissionView</t>
+          <t>CourseDetailView</t>
         </is>
       </c>
       <c r="K44" s="45" t="inlineStr">
@@ -32713,7 +32713,7 @@
       </c>
       <c r="M44" s="45" t="inlineStr">
         <is>
-          <t>提出物への合否、講評を送信。合格時は自動で次の教材を解禁。フィードバックはスレッドへ。</t>
+          <t>受講者別の課題進捗、未確認提出物、最終提出日時の一覧（image_32dcd7反映）。</t>
         </is>
       </c>
     </row>
@@ -32728,17 +32728,17 @@
       </c>
       <c r="C45" s="44" t="inlineStr">
         <is>
-          <t>/api/v1/instructor/courses/{courseId}/members</t>
+          <t>/api/v1/instructor/submissions/{submissionId}/evaluation</t>
         </is>
       </c>
       <c r="D45" s="43" t="inlineStr">
         <is>
-          <t>GET</t>
+          <t>PATCH</t>
         </is>
       </c>
       <c r="E45" s="44" t="inlineStr">
         <is>
-          <t>受講者名簿取得</t>
+          <t>評価・採点実行</t>
         </is>
       </c>
       <c r="F45" s="43" t="inlineStr">
@@ -32748,22 +32748,22 @@
       </c>
       <c r="G45" s="44" t="inlineStr">
         <is>
-          <t>instructor</t>
+          <t>instructor, assistant</t>
         </is>
       </c>
       <c r="H45" s="43" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>THREAD_REPLY(AUTO)</t>
         </is>
       </c>
       <c r="I45" s="45" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>GenericWriteRequest</t>
         </is>
       </c>
       <c r="J45" s="45" t="inlineStr">
         <is>
-          <t>CourseDetailView</t>
+          <t>SubmissionView</t>
         </is>
       </c>
       <c r="K45" s="45" t="inlineStr">
@@ -32778,7 +32778,7 @@
       </c>
       <c r="M45" s="45" t="inlineStr">
         <is>
-          <t>全参加ユーザーの属性、現在の進捗状況、メールアドレス等の名簿取得。</t>
+          <t>提出物への合否、講評を送信。合格時は自動で次の教材を解禁。フィードバックはスレッドへ。</t>
         </is>
       </c>
     </row>
@@ -32793,17 +32793,17 @@
       </c>
       <c r="C46" s="44" t="inlineStr">
         <is>
-          <t>/api/v1/instructor/courses/{courseId}/members/{userId}/role</t>
+          <t>/api/v1/instructor/courses/{courseId}/members</t>
         </is>
       </c>
       <c r="D46" s="43" t="inlineStr">
         <is>
-          <t>PATCH</t>
+          <t>GET</t>
         </is>
       </c>
       <c r="E46" s="44" t="inlineStr">
         <is>
-          <t>講座内ロール変更</t>
+          <t>受講者名簿取得</t>
         </is>
       </c>
       <c r="F46" s="43" t="inlineStr">
@@ -32813,17 +32813,17 @@
       </c>
       <c r="G46" s="44" t="inlineStr">
         <is>
-          <t>instructor_owner</t>
+          <t>instructor</t>
         </is>
       </c>
       <c r="H46" s="43" t="inlineStr">
         <is>
-          <t>423_ON_FROZEN</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I46" s="45" t="inlineStr">
         <is>
-          <t>GenericWriteRequest</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J46" s="45" t="inlineStr">
@@ -32833,7 +32833,7 @@
       </c>
       <c r="K46" s="45" t="inlineStr">
         <is>
-          <t>200, 423</t>
+          <t>200</t>
         </is>
       </c>
       <c r="L46" s="45" t="inlineStr">
@@ -32843,7 +32843,7 @@
       </c>
       <c r="M46" s="45" t="inlineStr">
         <is>
-          <t>特定ユーザーの役割（講師、アシスタント、受講生）を動的に切り替え。</t>
+          <t>全参加ユーザーの属性、現在の進捗状況、メールアドレス等の名簿取得。</t>
         </is>
       </c>
     </row>
@@ -32858,17 +32858,17 @@
       </c>
       <c r="C47" s="44" t="inlineStr">
         <is>
-          <t>/api/v1/instructor/courses/{courseId}/members/{userId}/revoke</t>
+          <t>/api/v1/instructor/courses/{courseId}/members/{userId}/role</t>
         </is>
       </c>
       <c r="D47" s="43" t="inlineStr">
         <is>
-          <t>POST</t>
+          <t>PATCH</t>
         </is>
       </c>
       <c r="E47" s="44" t="inlineStr">
         <is>
-          <t>受講権限剥奪</t>
+          <t>講座内ロール変更</t>
         </is>
       </c>
       <c r="F47" s="43" t="inlineStr">
@@ -32898,7 +32898,7 @@
       </c>
       <c r="K47" s="45" t="inlineStr">
         <is>
-          <t>201, 423</t>
+          <t>200, 423</t>
         </is>
       </c>
       <c r="L47" s="45" t="inlineStr">
@@ -32908,7 +32908,7 @@
       </c>
       <c r="M47" s="45" t="inlineStr">
         <is>
-          <t>特定ユーザーの受講権限を剥奪（revoked）し、コンテンツへのアクセスを遮断。</t>
+          <t>特定ユーザーの役割（講師、アシスタント、受講生）を動的に切り替え。</t>
         </is>
       </c>
     </row>
@@ -32923,17 +32923,17 @@
       </c>
       <c r="C48" s="44" t="inlineStr">
         <is>
-          <t>/api/v1/instructor/courses/{courseId}/export</t>
+          <t>/api/v1/instructor/courses/{courseId}/members/{userId}/revoke</t>
         </is>
       </c>
       <c r="D48" s="43" t="inlineStr">
         <is>
-          <t>GET</t>
+          <t>POST</t>
         </is>
       </c>
       <c r="E48" s="44" t="inlineStr">
         <is>
-          <t>受講者CSV出力</t>
+          <t>受講権限剥奪</t>
         </is>
       </c>
       <c r="F48" s="43" t="inlineStr">
@@ -32948,12 +32948,12 @@
       </c>
       <c r="H48" s="43" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>423_ON_FROZEN</t>
         </is>
       </c>
       <c r="I48" s="45" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>GenericWriteRequest</t>
         </is>
       </c>
       <c r="J48" s="45" t="inlineStr">
@@ -32963,7 +32963,7 @@
       </c>
       <c r="K48" s="45" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>201, 423</t>
         </is>
       </c>
       <c r="L48" s="45" t="inlineStr">
@@ -32973,7 +32973,7 @@
       </c>
       <c r="M48" s="45" t="inlineStr">
         <is>
-          <t>受講者名簿と学習進捗データをCSV形式でエクスポートする。</t>
+          <t>特定ユーザーの受講権限を剥奪（revoked）し、コンテンツへのアクセスを遮断。</t>
         </is>
       </c>
     </row>
@@ -32988,7 +32988,7 @@
       </c>
       <c r="C49" s="44" t="inlineStr">
         <is>
-          <t>/api/v1/courses/{courseId}/channels</t>
+          <t>/api/v1/instructor/courses/{courseId}/export</t>
         </is>
       </c>
       <c r="D49" s="43" t="inlineStr">
@@ -32998,7 +32998,7 @@
       </c>
       <c r="E49" s="44" t="inlineStr">
         <is>
-          <t>チャンネル一覧取得</t>
+          <t>受講者CSV出力</t>
         </is>
       </c>
       <c r="F49" s="43" t="inlineStr">
@@ -33008,7 +33008,7 @@
       </c>
       <c r="G49" s="44" t="inlineStr">
         <is>
-          <t>all_in_course</t>
+          <t>instructor_owner</t>
         </is>
       </c>
       <c r="H49" s="43" t="inlineStr">
@@ -33023,7 +33023,7 @@
       </c>
       <c r="J49" s="45" t="inlineStr">
         <is>
-          <t>CourseChannelListResponse</t>
+          <t>CourseDetailView</t>
         </is>
       </c>
       <c r="K49" s="45" t="inlineStr">
@@ -33038,7 +33038,7 @@
       </c>
       <c r="M49" s="45" t="inlineStr">
         <is>
-          <t>サイドメニュー構築用。general, announcement等のチャンネル種別を含む。</t>
+          <t>受講者名簿と学習進捗データをCSV形式でエクスポートする。</t>
         </is>
       </c>
     </row>
@@ -33058,12 +33058,12 @@
       </c>
       <c r="D50" s="43" t="inlineStr">
         <is>
-          <t>POST</t>
+          <t>GET</t>
         </is>
       </c>
       <c r="E50" s="44" t="inlineStr">
         <is>
-          <t>チャンネル作成</t>
+          <t>チャンネル一覧取得</t>
         </is>
       </c>
       <c r="F50" s="43" t="inlineStr">
@@ -33073,27 +33073,27 @@
       </c>
       <c r="G50" s="44" t="inlineStr">
         <is>
-          <t>instructor_owner</t>
+          <t>all_in_course</t>
         </is>
       </c>
       <c r="H50" s="43" t="inlineStr">
         <is>
-          <t>423_ON_FROZEN</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I50" s="45" t="inlineStr">
         <is>
-          <t>CourseChannelCreateRequest</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J50" s="45" t="inlineStr">
         <is>
-          <t>CourseDetailView</t>
+          <t>CourseChannelListResponse</t>
         </is>
       </c>
       <c r="K50" s="45" t="inlineStr">
         <is>
-          <t>201, 423</t>
+          <t>200</t>
         </is>
       </c>
       <c r="L50" s="45" t="inlineStr">
@@ -33103,7 +33103,7 @@
       </c>
       <c r="M50" s="45" t="inlineStr">
         <is>
-          <t>コース内に新しいカスタムチャンネルを追加。</t>
+          <t>サイドメニュー構築用。general, announcement等のチャンネル種別を含む。</t>
         </is>
       </c>
     </row>
@@ -33118,17 +33118,17 @@
       </c>
       <c r="C51" s="44" t="inlineStr">
         <is>
-          <t>/api/v1/channels/{channelId}</t>
+          <t>/api/v1/courses/{courseId}/channels</t>
         </is>
       </c>
       <c r="D51" s="43" t="inlineStr">
         <is>
-          <t>PUT</t>
+          <t>POST</t>
         </is>
       </c>
       <c r="E51" s="44" t="inlineStr">
         <is>
-          <t>チャンネル編集</t>
+          <t>チャンネル作成</t>
         </is>
       </c>
       <c r="F51" s="43" t="inlineStr">
@@ -33148,17 +33148,17 @@
       </c>
       <c r="I51" s="45" t="inlineStr">
         <is>
-          <t>GenericWriteRequest</t>
+          <t>CourseChannelCreateRequest</t>
         </is>
       </c>
       <c r="J51" s="45" t="inlineStr">
         <is>
-          <t>CourseChannelDetailView</t>
+          <t>CourseDetailView</t>
         </is>
       </c>
       <c r="K51" s="45" t="inlineStr">
         <is>
-          <t>200, 423</t>
+          <t>201, 423</t>
         </is>
       </c>
       <c r="L51" s="45" t="inlineStr">
@@ -33168,7 +33168,7 @@
       </c>
       <c r="M51" s="45" t="inlineStr">
         <is>
-          <t>チャンネル名、説明文、閲覧制限、アーカイブ状態の更新。</t>
+          <t>コース内に新しいカスタムチャンネルを追加。</t>
         </is>
       </c>
     </row>
@@ -33188,12 +33188,12 @@
       </c>
       <c r="D52" s="43" t="inlineStr">
         <is>
-          <t>DELETE</t>
+          <t>PUT</t>
         </is>
       </c>
       <c r="E52" s="44" t="inlineStr">
         <is>
-          <t>チャンネル削除</t>
+          <t>チャンネル編集</t>
         </is>
       </c>
       <c r="F52" s="43" t="inlineStr">
@@ -33213,12 +33213,12 @@
       </c>
       <c r="I52" s="45" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>GenericWriteRequest</t>
         </is>
       </c>
       <c r="J52" s="45" t="inlineStr">
         <is>
-          <t>SuccessResponse</t>
+          <t>CourseChannelDetailView</t>
         </is>
       </c>
       <c r="K52" s="45" t="inlineStr">
@@ -33233,7 +33233,7 @@
       </c>
       <c r="M52" s="45" t="inlineStr">
         <is>
-          <t>チャンネルを論理削除。過去ログは監査用に保持。</t>
+          <t>チャンネル名、説明文、閲覧制限、アーカイブ状態の更新。</t>
         </is>
       </c>
     </row>
@@ -33248,17 +33248,17 @@
       </c>
       <c r="C53" s="44" t="inlineStr">
         <is>
-          <t>/api/v1/channels/{channelId}/messages</t>
+          <t>/api/v1/channels/{channelId}</t>
         </is>
       </c>
       <c r="D53" s="43" t="inlineStr">
         <is>
-          <t>GET</t>
+          <t>DELETE</t>
         </is>
       </c>
       <c r="E53" s="44" t="inlineStr">
         <is>
-          <t>メッセージ履歴取得</t>
+          <t>チャンネル削除</t>
         </is>
       </c>
       <c r="F53" s="43" t="inlineStr">
@@ -33268,12 +33268,12 @@
       </c>
       <c r="G53" s="44" t="inlineStr">
         <is>
-          <t>all_in_course</t>
+          <t>instructor_owner</t>
         </is>
       </c>
       <c r="H53" s="43" t="inlineStr">
         <is>
-          <t>閲覧のみ可</t>
+          <t>423_ON_FROZEN</t>
         </is>
       </c>
       <c r="I53" s="45" t="inlineStr">
@@ -33283,12 +33283,12 @@
       </c>
       <c r="J53" s="45" t="inlineStr">
         <is>
-          <t>MessageListResponse</t>
+          <t>SuccessResponse</t>
         </is>
       </c>
       <c r="K53" s="45" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>200, 423</t>
         </is>
       </c>
       <c r="L53" s="45" t="inlineStr">
@@ -33298,7 +33298,7 @@
       </c>
       <c r="M53" s="45" t="inlineStr">
         <is>
-          <t>スレッド親（ルート）メッセージの一覧取得。課題の相互閲覧可（image_32d9b1反映）。</t>
+          <t>チャンネルを論理削除。過去ログは監査用に保持。</t>
         </is>
       </c>
     </row>
@@ -33318,12 +33318,12 @@
       </c>
       <c r="D54" s="43" t="inlineStr">
         <is>
-          <t>POST</t>
+          <t>GET</t>
         </is>
       </c>
       <c r="E54" s="44" t="inlineStr">
         <is>
-          <t>メッセージ投稿</t>
+          <t>メッセージ履歴取得</t>
         </is>
       </c>
       <c r="F54" s="43" t="inlineStr">
@@ -33338,22 +33338,22 @@
       </c>
       <c r="H54" s="43" t="inlineStr">
         <is>
-          <t>threads_only(AUTO)</t>
+          <t>閲覧のみ可</t>
         </is>
       </c>
       <c r="I54" s="45" t="inlineStr">
         <is>
-          <t>CourseMessageCreateRequest</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J54" s="45" t="inlineStr">
         <is>
-          <t>CourseChannelDetailView</t>
+          <t>MessageListResponse</t>
         </is>
       </c>
       <c r="K54" s="45" t="inlineStr">
         <is>
-          <t>201</t>
+          <t>200</t>
         </is>
       </c>
       <c r="L54" s="45" t="inlineStr">
@@ -33363,7 +33363,7 @@
       </c>
       <c r="M54" s="45" t="inlineStr">
         <is>
-          <t>チャンネルへの新規投稿。親メッセージとして保存。threads_onlyを強制適用。</t>
+          <t>スレッド親（ルート）メッセージの一覧取得。課題の相互閲覧可（image_32d9b1反映）。</t>
         </is>
       </c>
     </row>
@@ -33378,17 +33378,17 @@
       </c>
       <c r="C55" s="44" t="inlineStr">
         <is>
-          <t>/api/v1/messages/{messageId}/thread</t>
+          <t>/api/v1/channels/{channelId}/messages</t>
         </is>
       </c>
       <c r="D55" s="43" t="inlineStr">
         <is>
-          <t>GET</t>
+          <t>POST</t>
         </is>
       </c>
       <c r="E55" s="44" t="inlineStr">
         <is>
-          <t>スレッド詳細取得</t>
+          <t>メッセージ投稿</t>
         </is>
       </c>
       <c r="F55" s="43" t="inlineStr">
@@ -33403,22 +33403,22 @@
       </c>
       <c r="H55" s="43" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>threads_only(AUTO)</t>
         </is>
       </c>
       <c r="I55" s="45" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>CourseMessageCreateRequest</t>
         </is>
       </c>
       <c r="J55" s="45" t="inlineStr">
         <is>
-          <t>GenericListResponse</t>
+          <t>CourseChannelDetailView</t>
         </is>
       </c>
       <c r="K55" s="45" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>201</t>
         </is>
       </c>
       <c r="L55" s="45" t="inlineStr">
@@ -33428,7 +33428,7 @@
       </c>
       <c r="M55" s="45" t="inlineStr">
         <is>
-          <t>特定メッセージに紐づく返信メッセージ一覧（スレッドビュー）を全件取得。</t>
+          <t>チャンネルへの新規投稿。親メッセージとして保存。threads_onlyを強制適用。</t>
         </is>
       </c>
     </row>
@@ -33443,17 +33443,17 @@
       </c>
       <c r="C56" s="44" t="inlineStr">
         <is>
-          <t>/api/v1/messages/{messageId}/replies</t>
+          <t>/api/v1/messages/{messageId}/thread</t>
         </is>
       </c>
       <c r="D56" s="43" t="inlineStr">
         <is>
-          <t>POST</t>
+          <t>GET</t>
         </is>
       </c>
       <c r="E56" s="44" t="inlineStr">
         <is>
-          <t>スレッド返信投稿</t>
+          <t>スレッド詳細取得</t>
         </is>
       </c>
       <c r="F56" s="43" t="inlineStr">
@@ -33468,22 +33468,22 @@
       </c>
       <c r="H56" s="43" t="inlineStr">
         <is>
-          <t>THREAD_REPLY</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I56" s="45" t="inlineStr">
         <is>
-          <t>GenericWriteRequest</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J56" s="45" t="inlineStr">
         <is>
-          <t>CourseMessageView</t>
+          <t>GenericListResponse</t>
         </is>
       </c>
       <c r="K56" s="45" t="inlineStr">
         <is>
-          <t>201</t>
+          <t>200</t>
         </is>
       </c>
       <c r="L56" s="45" t="inlineStr">
@@ -33493,7 +33493,7 @@
       </c>
       <c r="M56" s="45" t="inlineStr">
         <is>
-          <t>返信投稿(image_32d9b1)。announcementタイプは講師以外返信不可。</t>
+          <t>特定メッセージに紐づく返信メッセージ一覧（スレッドビュー）を全件取得。</t>
         </is>
       </c>
     </row>
@@ -33508,17 +33508,17 @@
       </c>
       <c r="C57" s="44" t="inlineStr">
         <is>
-          <t>/api/v1/messages/{messageId}</t>
+          <t>/api/v1/messages/{messageId}/replies</t>
         </is>
       </c>
       <c r="D57" s="43" t="inlineStr">
         <is>
-          <t>PATCH</t>
+          <t>POST</t>
         </is>
       </c>
       <c r="E57" s="44" t="inlineStr">
         <is>
-          <t>メッセージ編集</t>
+          <t>スレッド返信投稿</t>
         </is>
       </c>
       <c r="F57" s="43" t="inlineStr">
@@ -33528,12 +33528,12 @@
       </c>
       <c r="G57" s="44" t="inlineStr">
         <is>
-          <t>owner_only</t>
+          <t>all_in_course</t>
         </is>
       </c>
       <c r="H57" s="43" t="inlineStr">
         <is>
-          <t>423_ON_FROZEN</t>
+          <t>THREAD_REPLY</t>
         </is>
       </c>
       <c r="I57" s="45" t="inlineStr">
@@ -33548,7 +33548,7 @@
       </c>
       <c r="K57" s="45" t="inlineStr">
         <is>
-          <t>200, 423</t>
+          <t>201</t>
         </is>
       </c>
       <c r="L57" s="45" t="inlineStr">
@@ -33558,7 +33558,7 @@
       </c>
       <c r="M57" s="45" t="inlineStr">
         <is>
-          <t>自分の投稿内容を修正。編集履歴を保持。423チェック対象。</t>
+          <t>返信投稿(image_32d9b1)。announcementタイプは講師以外返信不可。</t>
         </is>
       </c>
     </row>
@@ -33578,12 +33578,12 @@
       </c>
       <c r="D58" s="43" t="inlineStr">
         <is>
-          <t>DELETE</t>
+          <t>PATCH</t>
         </is>
       </c>
       <c r="E58" s="44" t="inlineStr">
         <is>
-          <t>メッセージ削除</t>
+          <t>メッセージ編集</t>
         </is>
       </c>
       <c r="F58" s="43" t="inlineStr">
@@ -33593,7 +33593,7 @@
       </c>
       <c r="G58" s="44" t="inlineStr">
         <is>
-          <t>owner_only, instructor</t>
+          <t>owner_only</t>
         </is>
       </c>
       <c r="H58" s="43" t="inlineStr">
@@ -33603,12 +33603,12 @@
       </c>
       <c r="I58" s="45" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>GenericWriteRequest</t>
         </is>
       </c>
       <c r="J58" s="45" t="inlineStr">
         <is>
-          <t>SuccessResponse</t>
+          <t>CourseMessageView</t>
         </is>
       </c>
       <c r="K58" s="45" t="inlineStr">
@@ -33623,7 +33623,7 @@
       </c>
       <c r="M58" s="45" t="inlineStr">
         <is>
-          <t>投稿の論理削除。返信がある場合は「削除されました」と表示。</t>
+          <t>自分の投稿内容を修正。編集履歴を保持。423チェック対象。</t>
         </is>
       </c>
     </row>
@@ -33638,17 +33638,17 @@
       </c>
       <c r="C59" s="44" t="inlineStr">
         <is>
-          <t>/api/v1/messages/{messageId}/reactions</t>
+          <t>/api/v1/messages/{messageId}</t>
         </is>
       </c>
       <c r="D59" s="43" t="inlineStr">
         <is>
-          <t>POST</t>
+          <t>DELETE</t>
         </is>
       </c>
       <c r="E59" s="44" t="inlineStr">
         <is>
-          <t>リアクション追加</t>
+          <t>メッセージ削除</t>
         </is>
       </c>
       <c r="F59" s="43" t="inlineStr">
@@ -33658,7 +33658,7 @@
       </c>
       <c r="G59" s="44" t="inlineStr">
         <is>
-          <t>all_in_course</t>
+          <t>owner_only, instructor</t>
         </is>
       </c>
       <c r="H59" s="43" t="inlineStr">
@@ -33668,17 +33668,17 @@
       </c>
       <c r="I59" s="45" t="inlineStr">
         <is>
-          <t>GenericWriteRequest</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J59" s="45" t="inlineStr">
         <is>
-          <t>CourseMessageView</t>
+          <t>SuccessResponse</t>
         </is>
       </c>
       <c r="K59" s="45" t="inlineStr">
         <is>
-          <t>201, 423</t>
+          <t>200, 423</t>
         </is>
       </c>
       <c r="L59" s="45" t="inlineStr">
@@ -33688,7 +33688,7 @@
       </c>
       <c r="M59" s="45" t="inlineStr">
         <is>
-          <t>メッセージに対する絵文字リアクションの付与。423チェック対象。</t>
+          <t>投稿の論理削除。返信がある場合は「削除されました」と表示。</t>
         </is>
       </c>
     </row>
@@ -33703,17 +33703,17 @@
       </c>
       <c r="C60" s="44" t="inlineStr">
         <is>
-          <t>/api/v1/courses/{courseId}/channels/{channelId}/threads</t>
+          <t>/api/v1/messages/{messageId}/reactions</t>
         </is>
       </c>
       <c r="D60" s="43" t="inlineStr">
         <is>
-          <t>GET</t>
+          <t>POST</t>
         </is>
       </c>
       <c r="E60" s="44" t="inlineStr">
         <is>
-          <t>スレッド一覧取得（ルートメッセージのみ）</t>
+          <t>リアクション追加</t>
         </is>
       </c>
       <c r="F60" s="43" t="inlineStr">
@@ -33728,22 +33728,22 @@
       </c>
       <c r="H60" s="43" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>423_ON_FROZEN</t>
         </is>
       </c>
       <c r="I60" s="45" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>GenericWriteRequest</t>
         </is>
       </c>
       <c r="J60" s="45" t="inlineStr">
         <is>
-          <t>ThreadListResponse</t>
+          <t>CourseMessageView</t>
         </is>
       </c>
       <c r="K60" s="45" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>201, 423</t>
         </is>
       </c>
       <c r="L60" s="45" t="inlineStr">
@@ -33753,7 +33753,7 @@
       </c>
       <c r="M60" s="45" t="inlineStr">
         <is>
-          <t>threads_only対応</t>
+          <t>メッセージに対する絵文字リアクションの付与。423チェック対象。</t>
         </is>
       </c>
     </row>
@@ -33773,12 +33773,12 @@
       </c>
       <c r="D61" s="43" t="inlineStr">
         <is>
-          <t>POST</t>
+          <t>GET</t>
         </is>
       </c>
       <c r="E61" s="44" t="inlineStr">
         <is>
-          <t>スレッド作成（ルート投稿）</t>
+          <t>スレッド一覧取得（ルートメッセージのみ）</t>
         </is>
       </c>
       <c r="F61" s="43" t="inlineStr">
@@ -33798,17 +33798,17 @@
       </c>
       <c r="I61" s="45" t="inlineStr">
         <is>
-          <t>GenericWriteRequest</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J61" s="45" t="inlineStr">
         <is>
-          <t>CourseDetailView</t>
+          <t>ThreadListResponse</t>
         </is>
       </c>
       <c r="K61" s="45" t="inlineStr">
         <is>
-          <t>201</t>
+          <t>200</t>
         </is>
       </c>
       <c r="L61" s="45" t="inlineStr">
@@ -33818,7 +33818,7 @@
       </c>
       <c r="M61" s="45" t="inlineStr">
         <is>
-          <t>threadId=NULLで作成</t>
+          <t>threads_only対応</t>
         </is>
       </c>
     </row>
@@ -33833,17 +33833,17 @@
       </c>
       <c r="C62" s="44" t="inlineStr">
         <is>
-          <t>/api/v1/courses/{courseId}/channels/{channelId}/threads/{threadId}/messages</t>
+          <t>/api/v1/courses/{courseId}/channels/{channelId}/threads</t>
         </is>
       </c>
       <c r="D62" s="43" t="inlineStr">
         <is>
-          <t>GET</t>
+          <t>POST</t>
         </is>
       </c>
       <c r="E62" s="44" t="inlineStr">
         <is>
-          <t>スレッド内メッセージ一覧（ルート+返信）</t>
+          <t>スレッド作成（ルート投稿）</t>
         </is>
       </c>
       <c r="F62" s="43" t="inlineStr">
@@ -33863,17 +33863,17 @@
       </c>
       <c r="I62" s="45" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>GenericWriteRequest</t>
         </is>
       </c>
       <c r="J62" s="45" t="inlineStr">
         <is>
-          <t>MessageListResponse</t>
+          <t>CourseDetailView</t>
         </is>
       </c>
       <c r="K62" s="45" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>201</t>
         </is>
       </c>
       <c r="L62" s="45" t="inlineStr">
@@ -33883,7 +33883,7 @@
       </c>
       <c r="M62" s="45" t="inlineStr">
         <is>
-          <t>threadId指定で返信も取得</t>
+          <t>threadId=NULLで作成</t>
         </is>
       </c>
     </row>
@@ -33903,12 +33903,12 @@
       </c>
       <c r="D63" s="43" t="inlineStr">
         <is>
-          <t>POST</t>
+          <t>GET</t>
         </is>
       </c>
       <c r="E63" s="44" t="inlineStr">
         <is>
-          <t>スレッド返信</t>
+          <t>スレッド内メッセージ一覧（ルート+返信）</t>
         </is>
       </c>
       <c r="F63" s="43" t="inlineStr">
@@ -33928,17 +33928,17 @@
       </c>
       <c r="I63" s="45" t="inlineStr">
         <is>
-          <t>CourseMessageCreateRequest</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J63" s="45" t="inlineStr">
         <is>
-          <t>CourseDetailView</t>
+          <t>MessageListResponse</t>
         </is>
       </c>
       <c r="K63" s="45" t="inlineStr">
         <is>
-          <t>201</t>
+          <t>200</t>
         </is>
       </c>
       <c r="L63" s="45" t="inlineStr">
@@ -33948,7 +33948,7 @@
       </c>
       <c r="M63" s="45" t="inlineStr">
         <is>
-          <t>threadId必須</t>
+          <t>threadId指定で返信も取得</t>
         </is>
       </c>
     </row>
@@ -33963,7 +33963,7 @@
       </c>
       <c r="C64" s="47" t="inlineStr">
         <is>
-          <t>/api/v1/payments/webhook</t>
+          <t>/api/v1/courses/{courseId}/channels/{channelId}/threads/{threadId}/messages</t>
         </is>
       </c>
       <c r="D64" s="46" t="inlineStr">
@@ -33973,7 +33973,7 @@
       </c>
       <c r="E64" s="47" t="inlineStr">
         <is>
-          <t>Stripe Webhook</t>
+          <t>スレッド返信</t>
         </is>
       </c>
       <c r="F64" s="46" t="inlineStr">
@@ -33983,27 +33983,27 @@
       </c>
       <c r="G64" s="47" t="inlineStr">
         <is>
-          <t>public(Stripe)</t>
+          <t>all_in_course</t>
         </is>
       </c>
       <c r="H64" s="46" t="inlineStr">
         <is>
-          <t>Webhook専用</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I64" s="45" t="inlineStr">
         <is>
-          <t>GenericWriteRequest</t>
+          <t>CourseMessageCreateRequest</t>
         </is>
       </c>
       <c r="J64" s="45" t="inlineStr">
         <is>
-          <t>SuccessResponse</t>
+          <t>CourseDetailView</t>
         </is>
       </c>
       <c r="K64" s="45" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>201</t>
         </is>
       </c>
       <c r="L64" s="45" t="inlineStr">
@@ -34013,7 +34013,7 @@
       </c>
       <c r="M64" s="45" t="inlineStr">
         <is>
-          <t>外部決済完了通知を受け取り、Enrollmentを自動的にactive化する。</t>
+          <t>threadId必須</t>
         </is>
       </c>
     </row>
@@ -34028,17 +34028,17 @@
       </c>
       <c r="C65" s="47" t="inlineStr">
         <is>
-          <t>/api/v1/health</t>
+          <t>/api/v1/payments/webhook</t>
         </is>
       </c>
       <c r="D65" s="46" t="inlineStr">
         <is>
-          <t>GET</t>
+          <t>POST</t>
         </is>
       </c>
       <c r="E65" s="47" t="inlineStr">
         <is>
-          <t>ヘルスチェック</t>
+          <t>Stripe Webhook</t>
         </is>
       </c>
       <c r="F65" s="46" t="inlineStr">
@@ -34048,22 +34048,22 @@
       </c>
       <c r="G65" s="47" t="inlineStr">
         <is>
-          <t>public</t>
+          <t>public(Stripe)</t>
         </is>
       </c>
       <c r="H65" s="46" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Webhook専用</t>
         </is>
       </c>
       <c r="I65" s="45" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>GenericWriteRequest</t>
         </is>
       </c>
       <c r="J65" s="45" t="inlineStr">
         <is>
-          <t>GenericListResponse</t>
+          <t>SuccessResponse</t>
         </is>
       </c>
       <c r="K65" s="45" t="inlineStr">
@@ -34078,7 +34078,7 @@
       </c>
       <c r="M65" s="45" t="inlineStr">
         <is>
-          <t>サーバーの死活監視用。DB、Redis、外部サービスの接続確認。</t>
+          <t>外部決済完了通知を受け取り、Enrollmentを自動的にactive化する。</t>
         </is>
       </c>
     </row>
@@ -34088,22 +34088,22 @@
       </c>
       <c r="B66" s="46" t="inlineStr">
         <is>
-          <t>API-031</t>
+          <t>API-065</t>
         </is>
       </c>
       <c r="C66" s="47" t="inlineStr">
         <is>
-          <t>/api/v1/instructor/courses/{courseId}/publish</t>
+          <t>/api/v1/health</t>
         </is>
       </c>
       <c r="D66" s="46" t="inlineStr">
         <is>
-          <t>POST</t>
+          <t>GET</t>
         </is>
       </c>
       <c r="E66" s="47" t="inlineStr">
         <is>
-          <t>コース公開（講師）</t>
+          <t>ヘルスチェック</t>
         </is>
       </c>
       <c r="F66" s="46" t="inlineStr">
@@ -34113,12 +34113,12 @@
       </c>
       <c r="G66" s="47" t="inlineStr">
         <is>
-          <t>instructor_owner</t>
+          <t>public</t>
         </is>
       </c>
       <c r="H66" s="46" t="inlineStr">
         <is>
-          <t>AUDIT_LOG</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I66" s="45" t="inlineStr">
@@ -34128,22 +34128,22 @@
       </c>
       <c r="J66" s="45" t="inlineStr">
         <is>
-          <t>CourseDetailView</t>
+          <t>GenericListResponse</t>
         </is>
       </c>
       <c r="K66" s="45" t="inlineStr">
         <is>
-          <t>200, 403, 423</t>
+          <t>200</t>
         </is>
       </c>
       <c r="L66" s="45" t="inlineStr">
         <is>
-          <t>v1.2</t>
+          <t>KEEP</t>
         </is>
       </c>
       <c r="M66" s="45" t="inlineStr">
         <is>
-          <t>ownerUserId一致の講師がコースを公開。statusをactiveに変更。operator作成コースの場合、CourseMember.role=instructor→instructor_ownerへ昇格（委譲完了）。</t>
+          <t>サーバーの死活監視用。DB、Redis、外部サービスの接続確認。</t>
         </is>
       </c>
     </row>

</xml_diff>